<commit_message>
corrected datum column in CoilSetup_ProtoMPEX.xlsx in Example 1
</commit_message>
<xml_diff>
--- a/Examples/Ex2 - ProtoMPEX/CoilSetup_ProtoMPEX.xlsx
+++ b/Examples/Ex2 - ProtoMPEX/CoilSetup_ProtoMPEX.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfc\Documents\LDRD_RfNeutronSource\MagneticFieldGeometry\MagneticFieldCode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfc\Documents\MATLAB\MyRepos\MagneticFieldCode_Axisymmetric\Examples\Ex4 - ProtoMPEX_FluxMapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD1D6C2-7D0C-48F6-BBED-0BE3E4A36E02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C71F91C-BBC9-4664-8398-363576F7CC74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{79EB1445-7373-446A-B7BC-60A0A49526E2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{79EB1445-7373-446A-B7BC-60A0A49526E2}"/>
   </bookViews>
   <sheets>
     <sheet name="conf_A" sheetId="1" r:id="rId1"/>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3E8440-D9FB-4112-AB41-3C415DE5C328}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1021,7 +1021,7 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0.98809999999999998</v>
@@ -1060,7 +1060,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1.2981</v>
@@ -1090,7 +1090,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1.6282000000000001</v>
@@ -1120,7 +1120,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>1.8642000000000001</v>
@@ -1150,7 +1150,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>2.1901999999999999</v>
@@ -1180,7 +1180,7 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>2.3881999999999999</v>
@@ -1210,7 +1210,7 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>2.9441999999999999</v>
@@ -1240,7 +1240,7 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>3.2201</v>
@@ -1270,7 +1270,7 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>3.4180999999999999</v>
@@ -1300,7 +1300,7 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>3.7342</v>
@@ -1330,7 +1330,7 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>4.0480999999999998</v>
@@ -1360,7 +1360,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>4.3662000000000001</v>
@@ -1391,7 +1391,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1447,7 +1447,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0.98809999999999998</v>
@@ -1486,7 +1486,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1.2981</v>
@@ -1516,7 +1516,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1.6282000000000001</v>
@@ -1546,7 +1546,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>1.8642000000000001</v>
@@ -1576,7 +1576,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>2.1901999999999999</v>
@@ -1606,7 +1606,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>2.3881999999999999</v>
@@ -1636,7 +1636,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>2.9441999999999999</v>
@@ -1666,7 +1666,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>3.2201</v>
@@ -1696,7 +1696,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>3.4180999999999999</v>
@@ -1726,7 +1726,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>3.7342</v>
@@ -1756,7 +1756,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>4.0480999999999998</v>
@@ -1786,7 +1786,7 @@
         <v>8</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>4.3662000000000001</v>
@@ -1817,7 +1817,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1873,7 +1873,7 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0.98809999999999998</v>
@@ -1912,7 +1912,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1.2981</v>
@@ -1942,7 +1942,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1.6282000000000001</v>
@@ -1972,7 +1972,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>1.8642000000000001</v>
@@ -2002,7 +2002,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>2.1901999999999999</v>
@@ -2032,7 +2032,7 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>2.3881999999999999</v>
@@ -2062,7 +2062,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>2.9441999999999999</v>
@@ -2092,7 +2092,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>3.1092</v>
@@ -2122,7 +2122,7 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>3.3887</v>
@@ -2152,7 +2152,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>3.5918999999999999</v>
@@ -2182,7 +2182,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>3.7824</v>
@@ -2212,7 +2212,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>3.9729000000000001</v>
@@ -2242,7 +2242,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <v>4.2904</v>
@@ -2329,7 +2329,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0.98809999999999998</v>
@@ -2368,7 +2368,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1.2981</v>
@@ -2398,7 +2398,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1.6282000000000001</v>
@@ -2428,7 +2428,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>1.8642000000000001</v>
@@ -2458,7 +2458,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>2.1901999999999999</v>
@@ -2488,7 +2488,7 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>2.3881999999999999</v>
@@ -2518,7 +2518,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>2.9441999999999999</v>
@@ -2548,7 +2548,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>3.1092</v>
@@ -2578,7 +2578,7 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>3.3887</v>
@@ -2608,7 +2608,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>3.5918999999999999</v>
@@ -2638,7 +2638,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>3.7824</v>
@@ -2668,7 +2668,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>3.9729000000000001</v>
@@ -2698,7 +2698,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <v>4.2904</v>
@@ -2728,8 +2728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C548EB1D-E9E6-4DD2-A63D-6AD4B7A9EEA6}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2785,7 +2785,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0.98809999999999998</v>
@@ -2824,7 +2824,7 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1.2981</v>
@@ -2854,7 +2854,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1.6282000000000001</v>
@@ -2884,7 +2884,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>1.8642000000000001</v>
@@ -2914,7 +2914,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>2.1901999999999999</v>
@@ -2944,7 +2944,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>2.3881999999999999</v>
@@ -2974,7 +2974,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>2.9441999999999999</v>
@@ -3004,7 +3004,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>3.1092</v>
@@ -3034,7 +3034,7 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>3.3887</v>
@@ -3064,7 +3064,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>3.5918999999999999</v>
@@ -3094,7 +3094,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>3.7824</v>
@@ -3124,7 +3124,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>3.9729000000000001</v>
@@ -3154,7 +3154,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <v>4.2904</v>
@@ -3185,7 +3185,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3241,7 +3241,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>0.98809999999999998</v>
@@ -3280,7 +3280,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1.2981</v>
@@ -3310,7 +3310,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1.6282000000000001</v>
@@ -3340,7 +3340,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>1.8642000000000001</v>
@@ -3370,7 +3370,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>2.1901999999999999</v>
@@ -3400,7 +3400,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>2.3881999999999999</v>
@@ -3430,7 +3430,7 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>2.9441999999999999</v>
@@ -3460,7 +3460,7 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>3.1092</v>
@@ -3490,7 +3490,7 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>3.3887</v>
@@ -3520,7 +3520,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>3.5918999999999999</v>
@@ -3550,7 +3550,7 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>3.7824</v>
@@ -3580,7 +3580,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>3.9729000000000001</v>
@@ -3610,7 +3610,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <v>4.2904</v>

</xml_diff>